<commit_message>
Moved cell ranges to parameters.txt
</commit_message>
<xml_diff>
--- a/input-FULL-v2.xlsx
+++ b/input-FULL-v2.xlsx
@@ -1,39 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fdiaz\Dropbox\Research\Papers\ONGOING_aa SMCE at SONGS (Journal of Environmental Management)\01-analysis\songs-evaluation-tool-master-6\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3A9D42-D459-4E31-A2A6-9B3887B28325}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="699" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24560" yWindow="100" windowWidth="24480" windowHeight="14480" tabRatio="699"/>
   </bookViews>
   <sheets>
     <sheet name="IMPACT-TECH" sheetId="10" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>François Diaz-Maurin</author>
   </authors>
   <commentList>
-    <comment ref="AE3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="AE3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -46,7 +40,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="AF3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="AG3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="79">
   <si>
     <t>Management</t>
   </si>
@@ -315,15 +309,12 @@
   </si>
   <si>
     <t>Public Safety</t>
-  </si>
-  <si>
-    <t>A3:AG25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -331,7 +322,7 @@
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,6 +367,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -442,14 +449,18 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -525,9 +536,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -559,9 +567,16 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -871,59 +886,57 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AH34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="81.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" style="2" customWidth="1"/>
-    <col min="7" max="8" width="7.28515625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" style="2" customWidth="1"/>
-    <col min="10" max="11" width="7.28515625" style="7" customWidth="1"/>
-    <col min="12" max="12" width="7.28515625" style="2" customWidth="1"/>
-    <col min="13" max="14" width="7.28515625" style="7" customWidth="1"/>
-    <col min="15" max="15" width="7.28515625" style="2" customWidth="1"/>
-    <col min="16" max="17" width="7.28515625" style="7" customWidth="1"/>
-    <col min="18" max="18" width="7.28515625" style="2" customWidth="1"/>
-    <col min="19" max="20" width="7.28515625" style="7" customWidth="1"/>
-    <col min="21" max="21" width="7.28515625" style="2" customWidth="1"/>
-    <col min="22" max="23" width="7.28515625" style="7" customWidth="1"/>
-    <col min="24" max="24" width="7.28515625" style="2" customWidth="1"/>
-    <col min="25" max="26" width="7.28515625" style="7" customWidth="1"/>
-    <col min="27" max="27" width="7.28515625" style="2" customWidth="1"/>
-    <col min="28" max="29" width="7.28515625" style="7" customWidth="1"/>
-    <col min="30" max="30" width="8.85546875" style="3"/>
-    <col min="31" max="33" width="12.140625" style="2" customWidth="1"/>
-    <col min="34" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="13.33203125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="81.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="2" customWidth="1"/>
+    <col min="7" max="8" width="7.33203125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" style="2" customWidth="1"/>
+    <col min="10" max="11" width="7.33203125" style="7" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" style="2" customWidth="1"/>
+    <col min="13" max="14" width="7.33203125" style="7" customWidth="1"/>
+    <col min="15" max="15" width="7.33203125" style="2" customWidth="1"/>
+    <col min="16" max="17" width="7.33203125" style="7" customWidth="1"/>
+    <col min="18" max="18" width="7.33203125" style="2" customWidth="1"/>
+    <col min="19" max="20" width="7.33203125" style="7" customWidth="1"/>
+    <col min="21" max="21" width="7.33203125" style="2" customWidth="1"/>
+    <col min="22" max="23" width="7.33203125" style="7" customWidth="1"/>
+    <col min="24" max="24" width="7.33203125" style="2" customWidth="1"/>
+    <col min="25" max="26" width="7.33203125" style="7" customWidth="1"/>
+    <col min="27" max="27" width="7.33203125" style="2" customWidth="1"/>
+    <col min="28" max="29" width="7.33203125" style="7" customWidth="1"/>
+    <col min="30" max="30" width="8.83203125" style="3"/>
+    <col min="31" max="33" width="12.1640625" style="2" customWidth="1"/>
+    <col min="34" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C1" s="16"/>
-      <c r="D1" s="17" t="s">
-        <v>79</v>
-      </c>
+      <c r="D1" s="17"/>
       <c r="F1" s="3"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
@@ -949,49 +962,49 @@
       <c r="AB1" s="8"/>
       <c r="AC1" s="8"/>
     </row>
-    <row r="2" spans="1:34" s="14" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F2" s="29" t="s">
+    <row r="2" spans="1:34" s="14" customFormat="1" ht="30.75" customHeight="1">
+      <c r="F2" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29" t="s">
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29" t="s">
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29" t="s">
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29" t="s">
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="29" t="s">
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="29"/>
-      <c r="W2" s="29"/>
-      <c r="X2" s="29" t="s">
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+      <c r="X2" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Y2" s="29"/>
-      <c r="Z2" s="29"/>
-      <c r="AA2" s="29" t="s">
+      <c r="Y2" s="40"/>
+      <c r="Z2" s="40"/>
+      <c r="AA2" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="AB2" s="29"/>
-      <c r="AC2" s="29"/>
+      <c r="AB2" s="40"/>
+      <c r="AC2" s="40"/>
     </row>
-    <row r="3" spans="1:34" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" s="1" customFormat="1" ht="28">
       <c r="A3" s="15" t="s">
         <v>42</v>
       </c>
@@ -1093,7 +1106,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34">
       <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
@@ -1194,7 +1207,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34">
       <c r="B5" s="11" t="s">
         <v>25</v>
       </c>
@@ -1292,7 +1305,7 @@
         <v>400.00000000000011</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34">
       <c r="B6" s="11" t="s">
         <v>26</v>
       </c>
@@ -1388,7 +1401,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34">
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
@@ -1484,7 +1497,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34">
       <c r="B8" s="11" t="s">
         <v>28</v>
       </c>
@@ -1580,7 +1593,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34">
       <c r="B9" s="11" t="s">
         <v>29</v>
       </c>
@@ -1676,7 +1689,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" ht="28">
       <c r="A10" s="9" t="s">
         <v>77</v>
       </c>
@@ -1777,7 +1790,7 @@
         <v>322.33425568694531</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34">
       <c r="B11" s="11" t="s">
         <v>31</v>
       </c>
@@ -1873,7 +1886,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34">
       <c r="B12" s="11" t="s">
         <v>32</v>
       </c>
@@ -1971,7 +1984,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34">
       <c r="B13" s="11" t="s">
         <v>33</v>
       </c>
@@ -2067,9 +2080,9 @@
         <v>400</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
-      <c r="B14" s="39" t="s">
+    <row r="14" spans="1:34">
+      <c r="A14" s="38"/>
+      <c r="B14" s="38" t="s">
         <v>34</v>
       </c>
       <c r="C14" s="11" t="s">
@@ -2164,7 +2177,7 @@
         <v>400.00000000000011</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34">
       <c r="A15" s="11" t="s">
         <v>78</v>
       </c>
@@ -2180,76 +2193,76 @@
       <c r="E15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="40">
+      <c r="F15" s="39">
         <v>200</v>
       </c>
-      <c r="G15" s="40">
+      <c r="G15" s="39">
         <v>200</v>
       </c>
-      <c r="H15" s="40">
+      <c r="H15" s="39">
         <v>200</v>
       </c>
-      <c r="I15" s="40">
+      <c r="I15" s="39">
         <v>30</v>
       </c>
-      <c r="J15" s="40">
+      <c r="J15" s="39">
         <v>20</v>
       </c>
-      <c r="K15" s="40">
+      <c r="K15" s="39">
         <v>40</v>
       </c>
-      <c r="L15" s="40">
+      <c r="L15" s="39">
         <v>30</v>
       </c>
-      <c r="M15" s="40">
+      <c r="M15" s="39">
         <v>20</v>
       </c>
-      <c r="N15" s="40">
+      <c r="N15" s="39">
         <v>40</v>
       </c>
-      <c r="O15" s="40">
+      <c r="O15" s="39">
         <v>60</v>
       </c>
-      <c r="P15" s="40">
+      <c r="P15" s="39">
         <v>20</v>
       </c>
-      <c r="Q15" s="40">
+      <c r="Q15" s="39">
         <v>100</v>
       </c>
-      <c r="R15" s="40">
+      <c r="R15" s="39">
         <v>60</v>
       </c>
-      <c r="S15" s="40">
+      <c r="S15" s="39">
         <v>20</v>
       </c>
-      <c r="T15" s="40">
+      <c r="T15" s="39">
         <v>100</v>
       </c>
-      <c r="U15" s="40">
+      <c r="U15" s="39">
         <v>30</v>
       </c>
-      <c r="V15" s="40">
+      <c r="V15" s="39">
         <v>20</v>
       </c>
-      <c r="W15" s="40">
+      <c r="W15" s="39">
         <v>40</v>
       </c>
-      <c r="X15" s="40">
+      <c r="X15" s="39">
         <v>30</v>
       </c>
-      <c r="Y15" s="40">
+      <c r="Y15" s="39">
         <v>20</v>
       </c>
-      <c r="Z15" s="40">
+      <c r="Z15" s="39">
         <v>40</v>
       </c>
-      <c r="AA15" s="40">
+      <c r="AA15" s="39">
         <v>30</v>
       </c>
-      <c r="AB15" s="40">
+      <c r="AB15" s="39">
         <v>20</v>
       </c>
-      <c r="AC15" s="40">
+      <c r="AC15" s="39">
         <v>40</v>
       </c>
       <c r="AE15" s="24">
@@ -2263,7 +2276,7 @@
         <v>267.76859504132233</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34">
       <c r="B16" s="11" t="s">
         <v>53</v>
       </c>
@@ -2359,7 +2372,7 @@
         <v>267.76859504132233</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34">
       <c r="B17" s="11">
         <v>2.2999999999999998</v>
       </c>
@@ -2369,7 +2382,7 @@
       <c r="D17" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="29" t="s">
         <v>56</v>
       </c>
       <c r="F17" s="19">
@@ -2447,7 +2460,7 @@
       <c r="AE17" s="22">
         <v>30</v>
       </c>
-      <c r="AF17" s="31"/>
+      <c r="AF17" s="30"/>
       <c r="AG17" s="22" t="b">
         <v>0</v>
       </c>
@@ -2455,7 +2468,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34">
       <c r="B18" s="11" t="s">
         <v>57</v>
       </c>
@@ -2468,76 +2481,76 @@
       <c r="E18" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="32">
+      <c r="F18" s="31">
         <v>9.9321112826514213</v>
       </c>
-      <c r="G18" s="32">
+      <c r="G18" s="31">
         <v>7.7567426067347807</v>
       </c>
-      <c r="H18" s="32">
+      <c r="H18" s="31">
         <v>13.126319087739748</v>
       </c>
-      <c r="I18" s="32">
+      <c r="I18" s="31">
         <v>1.693606752729711</v>
       </c>
-      <c r="J18" s="32">
+      <c r="J18" s="31">
         <v>1.1296107343160331</v>
       </c>
-      <c r="K18" s="32">
+      <c r="K18" s="31">
         <v>2.2576027711433886</v>
       </c>
-      <c r="L18" s="32">
+      <c r="L18" s="31">
         <v>1.693606752729711</v>
       </c>
-      <c r="M18" s="32">
+      <c r="M18" s="31">
         <v>1.1296107343160331</v>
       </c>
-      <c r="N18" s="32">
+      <c r="N18" s="31">
         <v>2.2576027711433886</v>
       </c>
-      <c r="O18" s="32">
+      <c r="O18" s="31">
         <v>3.0482713406259045</v>
       </c>
-      <c r="P18" s="32">
+      <c r="P18" s="31">
         <v>1.1296107343160331</v>
       </c>
-      <c r="Q18" s="32">
+      <c r="Q18" s="31">
         <v>5.4268186542917594</v>
       </c>
-      <c r="R18" s="32">
+      <c r="R18" s="31">
         <v>3.0482713406259045</v>
       </c>
-      <c r="S18" s="32">
+      <c r="S18" s="31">
         <v>1.1296107343160331</v>
       </c>
-      <c r="T18" s="32">
+      <c r="T18" s="31">
         <v>5.4268186542917594</v>
       </c>
-      <c r="U18" s="32">
+      <c r="U18" s="31">
         <v>1.693606752729711</v>
       </c>
-      <c r="V18" s="32">
+      <c r="V18" s="31">
         <v>1.1296107343160331</v>
       </c>
-      <c r="W18" s="32">
+      <c r="W18" s="31">
         <v>2.2576027711433886</v>
       </c>
-      <c r="X18" s="32">
+      <c r="X18" s="31">
         <v>1.693606752729711</v>
       </c>
-      <c r="Y18" s="32">
+      <c r="Y18" s="31">
         <v>1.1296107343160331</v>
       </c>
-      <c r="Z18" s="32">
+      <c r="Z18" s="31">
         <v>2.2576027711433886</v>
       </c>
-      <c r="AA18" s="32">
+      <c r="AA18" s="31">
         <v>1.693606752729711</v>
       </c>
-      <c r="AB18" s="32">
+      <c r="AB18" s="31">
         <v>1.1296107343160331</v>
       </c>
-      <c r="AC18" s="32">
+      <c r="AC18" s="31">
         <v>2.2576027711433886</v>
       </c>
       <c r="AE18" s="23">
@@ -2553,7 +2566,7 @@
         <v>283.26511680855992</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34">
       <c r="B19" s="11" t="s">
         <v>60</v>
       </c>
@@ -2584,58 +2597,58 @@
       <c r="K19" s="19">
         <v>10.594761322080478</v>
       </c>
-      <c r="L19" s="32">
+      <c r="L19" s="31">
         <v>2.1113720079402762</v>
       </c>
-      <c r="M19" s="32">
+      <c r="M19" s="31">
         <v>1.5429100491934944</v>
       </c>
-      <c r="N19" s="32">
+      <c r="N19" s="31">
         <v>2.6798339666870583</v>
       </c>
-      <c r="O19" s="32">
+      <c r="O19" s="31">
         <v>3.8018827612146211</v>
       </c>
-      <c r="P19" s="32">
+      <c r="P19" s="31">
         <v>1.5429100491934944</v>
       </c>
-      <c r="Q19" s="32">
+      <c r="Q19" s="31">
         <v>5.6356321148190061</v>
       </c>
-      <c r="R19" s="32">
+      <c r="R19" s="31">
         <v>3.8018827612146211</v>
       </c>
-      <c r="S19" s="32">
+      <c r="S19" s="31">
         <v>1.5429100491934944</v>
       </c>
-      <c r="T19" s="32">
+      <c r="T19" s="31">
         <v>5.6356321148190061</v>
       </c>
-      <c r="U19" s="32">
+      <c r="U19" s="31">
         <v>5.1771947764179096</v>
       </c>
-      <c r="V19" s="32">
+      <c r="V19" s="31">
         <v>2.6798339666870583</v>
       </c>
-      <c r="W19" s="32">
+      <c r="W19" s="31">
         <v>7.579159661637874</v>
       </c>
-      <c r="X19" s="32">
+      <c r="X19" s="31">
         <v>5.1771947764179096</v>
       </c>
-      <c r="Y19" s="32">
+      <c r="Y19" s="31">
         <v>2.6798339666870583</v>
       </c>
-      <c r="Z19" s="32">
+      <c r="Z19" s="31">
         <v>7.579159661637874</v>
       </c>
-      <c r="AA19" s="32">
+      <c r="AA19" s="31">
         <v>2.1113720079402762</v>
       </c>
-      <c r="AB19" s="32">
+      <c r="AB19" s="31">
         <v>1.5429100491934944</v>
       </c>
-      <c r="AC19" s="32">
+      <c r="AC19" s="31">
         <v>2.6798339666870583</v>
       </c>
       <c r="AE19" s="23">
@@ -2651,7 +2664,7 @@
         <v>222.46621256208954</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34">
       <c r="B20" s="11" t="s">
         <v>63</v>
       </c>
@@ -2673,70 +2686,70 @@
       <c r="H20" s="13">
         <v>0</v>
       </c>
-      <c r="I20" s="33">
+      <c r="I20" s="32">
         <v>2.8917910447761194E-2</v>
       </c>
-      <c r="J20" s="33">
+      <c r="J20" s="32">
         <v>3.0487804878048777E-3</v>
       </c>
-      <c r="K20" s="33">
+      <c r="K20" s="32">
         <v>0.10016025641025642</v>
       </c>
-      <c r="L20" s="33">
+      <c r="L20" s="32">
         <v>2.8917910447761194E-2</v>
       </c>
-      <c r="M20" s="33">
+      <c r="M20" s="32">
         <v>3.0487804878048777E-3</v>
       </c>
-      <c r="N20" s="33">
+      <c r="N20" s="32">
         <v>0.10016025641025642</v>
       </c>
-      <c r="O20" s="33">
+      <c r="O20" s="32">
         <v>2.8917910447761194E-2</v>
       </c>
-      <c r="P20" s="33">
+      <c r="P20" s="32">
         <v>3.0487804878048777E-3</v>
       </c>
-      <c r="Q20" s="33">
+      <c r="Q20" s="32">
         <v>0.10016025641025642</v>
       </c>
-      <c r="R20" s="33">
+      <c r="R20" s="32">
         <v>2.8917910447761194E-2</v>
       </c>
-      <c r="S20" s="33">
+      <c r="S20" s="32">
         <v>3.0487804878048777E-3</v>
       </c>
-      <c r="T20" s="33">
+      <c r="T20" s="32">
         <v>0.10016025641025642</v>
       </c>
-      <c r="U20" s="33">
+      <c r="U20" s="32">
         <v>5.7835820895522388E-2</v>
       </c>
-      <c r="V20" s="33">
+      <c r="V20" s="32">
         <v>6.0975609756097554E-3</v>
       </c>
-      <c r="W20" s="33">
+      <c r="W20" s="32">
         <v>0.20032051282051283</v>
       </c>
-      <c r="X20" s="33">
+      <c r="X20" s="32">
         <v>5.7835820895522388E-2</v>
       </c>
-      <c r="Y20" s="33">
+      <c r="Y20" s="32">
         <v>6.0975609756097554E-3</v>
       </c>
-      <c r="Z20" s="33">
+      <c r="Z20" s="32">
         <v>0.20032051282051283</v>
       </c>
-      <c r="AA20" s="33">
+      <c r="AA20" s="32">
         <v>5.7835820895522388E-2</v>
       </c>
-      <c r="AB20" s="33">
+      <c r="AB20" s="32">
         <v>6.0975609756097554E-3</v>
       </c>
-      <c r="AC20" s="33">
+      <c r="AC20" s="32">
         <v>0.20032051282051283</v>
       </c>
-      <c r="AE20" s="34">
+      <c r="AE20" s="33">
         <v>3.3386752136752136E-2</v>
       </c>
       <c r="AF20" s="11"/>
@@ -2747,7 +2760,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34">
       <c r="A21" s="9" t="s">
         <v>66</v>
       </c>
@@ -2763,76 +2776,76 @@
       <c r="E21" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="35">
+      <c r="F21" s="34">
         <v>2270.6</v>
       </c>
-      <c r="G21" s="35">
+      <c r="G21" s="34">
         <v>2135.3000000000002</v>
       </c>
-      <c r="H21" s="35">
+      <c r="H21" s="34">
         <v>2541.1999999999998</v>
       </c>
-      <c r="I21" s="35">
+      <c r="I21" s="34">
         <v>300</v>
       </c>
-      <c r="J21" s="35">
+      <c r="J21" s="34">
         <v>200</v>
       </c>
-      <c r="K21" s="35">
+      <c r="K21" s="34">
         <v>496.8</v>
       </c>
-      <c r="L21" s="35">
+      <c r="L21" s="34">
         <v>300</v>
       </c>
-      <c r="M21" s="35">
+      <c r="M21" s="34">
         <v>200</v>
       </c>
-      <c r="N21" s="35">
+      <c r="N21" s="34">
         <v>496.8</v>
       </c>
-      <c r="O21" s="35">
+      <c r="O21" s="34">
         <v>606.6</v>
       </c>
-      <c r="P21" s="35">
+      <c r="P21" s="34">
         <v>200</v>
       </c>
-      <c r="Q21" s="35">
+      <c r="Q21" s="34">
         <v>1270.5999999999999</v>
       </c>
-      <c r="R21" s="35">
+      <c r="R21" s="34">
         <v>606.6</v>
       </c>
-      <c r="S21" s="35">
+      <c r="S21" s="34">
         <v>200</v>
       </c>
-      <c r="T21" s="35">
+      <c r="T21" s="34">
         <v>1270.5999999999999</v>
       </c>
-      <c r="U21" s="35">
+      <c r="U21" s="34">
         <v>300</v>
       </c>
-      <c r="V21" s="35">
+      <c r="V21" s="34">
         <v>200</v>
       </c>
-      <c r="W21" s="35">
+      <c r="W21" s="34">
         <v>496.8</v>
       </c>
-      <c r="X21" s="35">
+      <c r="X21" s="34">
         <v>300</v>
       </c>
-      <c r="Y21" s="35">
+      <c r="Y21" s="34">
         <v>200</v>
       </c>
-      <c r="Z21" s="35">
+      <c r="Z21" s="34">
         <v>496.8</v>
       </c>
-      <c r="AA21" s="35">
+      <c r="AA21" s="34">
         <v>300</v>
       </c>
-      <c r="AB21" s="35">
+      <c r="AB21" s="34">
         <v>200</v>
       </c>
-      <c r="AC21" s="35">
+      <c r="AC21" s="34">
         <v>496.8</v>
       </c>
       <c r="AE21" s="24">
@@ -2848,7 +2861,7 @@
         <v>291.78003760315778</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34">
       <c r="B22" s="11">
         <v>2.8</v>
       </c>
@@ -2861,76 +2874,76 @@
       <c r="E22" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="36">
-        <v>0</v>
-      </c>
-      <c r="G22" s="36">
-        <v>0</v>
-      </c>
-      <c r="H22" s="36">
-        <v>0</v>
-      </c>
-      <c r="I22" s="36">
+      <c r="F22" s="35">
+        <v>0</v>
+      </c>
+      <c r="G22" s="35">
+        <v>0</v>
+      </c>
+      <c r="H22" s="35">
+        <v>0</v>
+      </c>
+      <c r="I22" s="35">
         <v>2241.1883561643835</v>
       </c>
-      <c r="J22" s="36">
+      <c r="J22" s="35">
         <v>2005.9383561643835</v>
       </c>
-      <c r="K22" s="36">
+      <c r="K22" s="35">
         <v>2610.6675228310505</v>
       </c>
-      <c r="L22" s="36">
-        <v>0</v>
-      </c>
-      <c r="M22" s="36">
-        <v>0</v>
-      </c>
-      <c r="N22" s="36">
-        <v>0</v>
-      </c>
-      <c r="O22" s="36">
+      <c r="L22" s="35">
+        <v>0</v>
+      </c>
+      <c r="M22" s="35">
+        <v>0</v>
+      </c>
+      <c r="N22" s="35">
+        <v>0</v>
+      </c>
+      <c r="O22" s="35">
         <v>656.73922500000003</v>
       </c>
-      <c r="P22" s="36">
+      <c r="P22" s="35">
         <v>287.28750000000002</v>
       </c>
-      <c r="Q22" s="36">
+      <c r="Q22" s="35">
         <v>1333.0139999999999</v>
       </c>
-      <c r="R22" s="36">
-        <v>0</v>
-      </c>
-      <c r="S22" s="36">
-        <v>0</v>
-      </c>
-      <c r="T22" s="36">
-        <v>0</v>
-      </c>
-      <c r="U22" s="36">
+      <c r="R22" s="35">
+        <v>0</v>
+      </c>
+      <c r="S22" s="35">
+        <v>0</v>
+      </c>
+      <c r="T22" s="35">
+        <v>0</v>
+      </c>
+      <c r="U22" s="35">
         <v>1536.8775811643836</v>
       </c>
-      <c r="V22" s="36">
+      <c r="V22" s="35">
         <v>761.4258561643835</v>
       </c>
-      <c r="W22" s="36">
+      <c r="W22" s="35">
         <v>2901.5815228310503</v>
       </c>
-      <c r="X22" s="36">
+      <c r="X22" s="35">
         <v>880.13835616438359</v>
       </c>
-      <c r="Y22" s="36">
+      <c r="Y22" s="35">
         <v>474.13835616438354</v>
       </c>
-      <c r="Z22" s="36">
+      <c r="Z22" s="35">
         <v>1568.5675228310502</v>
       </c>
-      <c r="AA22" s="36">
-        <v>0</v>
-      </c>
-      <c r="AB22" s="36">
-        <v>0</v>
-      </c>
-      <c r="AC22" s="36">
+      <c r="AA22" s="35">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="35">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="35">
         <v>0</v>
       </c>
       <c r="AE22" s="22">
@@ -2944,7 +2957,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34">
       <c r="B23" s="11" t="s">
         <v>71</v>
       </c>
@@ -2957,76 +2970,76 @@
       <c r="E23" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="36">
-        <v>0</v>
-      </c>
-      <c r="G23" s="36">
-        <v>0</v>
-      </c>
-      <c r="H23" s="36">
-        <v>0</v>
-      </c>
-      <c r="I23" s="37">
+      <c r="F23" s="35">
+        <v>0</v>
+      </c>
+      <c r="G23" s="35">
+        <v>0</v>
+      </c>
+      <c r="H23" s="35">
+        <v>0</v>
+      </c>
+      <c r="I23" s="36">
         <v>6.6497816352588943</v>
       </c>
-      <c r="J23" s="36">
-        <v>0</v>
-      </c>
-      <c r="K23" s="36">
+      <c r="J23" s="35">
+        <v>0</v>
+      </c>
+      <c r="K23" s="35">
         <v>11.496319126452976</v>
       </c>
-      <c r="L23" s="36">
+      <c r="L23" s="35">
         <v>11.220132987701069</v>
       </c>
-      <c r="M23" s="37">
+      <c r="M23" s="36">
         <v>3.4094245332863689</v>
       </c>
-      <c r="N23" s="36">
+      <c r="N23" s="35">
         <v>21.142655864741108</v>
       </c>
-      <c r="O23" s="37">
+      <c r="O23" s="36">
         <v>7.5565700400669256</v>
       </c>
-      <c r="P23" s="37">
+      <c r="P23" s="36">
         <v>3.6367195021721268</v>
       </c>
-      <c r="Q23" s="36">
+      <c r="Q23" s="35">
         <v>11.496319126452976</v>
       </c>
-      <c r="R23" s="37">
+      <c r="R23" s="36">
         <v>6.0416100703005764</v>
       </c>
-      <c r="S23" s="37">
+      <c r="S23" s="36">
         <v>3.4094245332863689</v>
       </c>
-      <c r="T23" s="37">
+      <c r="T23" s="36">
         <v>8.4570623458964427</v>
       </c>
-      <c r="U23" s="37">
+      <c r="U23" s="36">
         <v>5.9121155666607965</v>
       </c>
-      <c r="V23" s="37">
+      <c r="V23" s="36">
         <v>4.3512386990724439</v>
       </c>
-      <c r="W23" s="37">
+      <c r="W23" s="36">
         <v>8.9520517787953491</v>
       </c>
-      <c r="X23" s="37">
+      <c r="X23" s="36">
         <v>4.2165083184599688</v>
       </c>
-      <c r="Y23" s="37">
+      <c r="Y23" s="36">
         <v>2.362283273839878</v>
       </c>
-      <c r="Z23" s="37">
+      <c r="Z23" s="36">
         <v>5.7805609382967873</v>
       </c>
-      <c r="AA23" s="36">
+      <c r="AA23" s="35">
         <v>14.693892624936256</v>
       </c>
-      <c r="AB23" s="37">
+      <c r="AB23" s="36">
         <v>1.7876083630800612</v>
       </c>
-      <c r="AC23" s="36">
+      <c r="AC23" s="35">
         <v>32.114227434982148</v>
       </c>
       <c r="AE23" s="23">
@@ -3040,7 +3053,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="24" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34">
       <c r="B24" s="11" t="s">
         <v>73</v>
       </c>
@@ -3050,79 +3063,79 @@
       <c r="D24" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="30" t="s">
+      <c r="E24" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="F24" s="36">
+      <c r="F24" s="35">
         <v>4826.4299999999994</v>
       </c>
-      <c r="G24" s="36">
-        <v>0</v>
-      </c>
-      <c r="H24" s="36">
+      <c r="G24" s="35">
+        <v>0</v>
+      </c>
+      <c r="H24" s="35">
         <v>4826.4299999999994</v>
       </c>
-      <c r="I24" s="36">
+      <c r="I24" s="35">
         <v>723.96449999999982</v>
       </c>
-      <c r="J24" s="36">
-        <v>0</v>
-      </c>
-      <c r="K24" s="36">
+      <c r="J24" s="35">
+        <v>0</v>
+      </c>
+      <c r="K24" s="35">
         <v>4826.4299999999994</v>
       </c>
-      <c r="L24" s="36">
+      <c r="L24" s="35">
         <v>723.96449999999982</v>
       </c>
-      <c r="M24" s="36">
-        <v>0</v>
-      </c>
-      <c r="N24" s="36">
+      <c r="M24" s="35">
+        <v>0</v>
+      </c>
+      <c r="N24" s="35">
         <v>965.28599999999983</v>
       </c>
-      <c r="O24" s="36">
+      <c r="O24" s="35">
         <v>1447.9289999999996</v>
       </c>
-      <c r="P24" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="36">
+      <c r="P24" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="35">
         <v>2413.2149999999997</v>
       </c>
-      <c r="R24" s="36">
+      <c r="R24" s="35">
         <v>1447.9289999999996</v>
       </c>
-      <c r="S24" s="36">
-        <v>0</v>
-      </c>
-      <c r="T24" s="36">
+      <c r="S24" s="35">
+        <v>0</v>
+      </c>
+      <c r="T24" s="35">
         <v>2413.2149999999997</v>
       </c>
-      <c r="U24" s="36">
+      <c r="U24" s="35">
         <v>723.96449999999982</v>
       </c>
-      <c r="V24" s="36">
-        <v>0</v>
-      </c>
-      <c r="W24" s="36">
+      <c r="V24" s="35">
+        <v>0</v>
+      </c>
+      <c r="W24" s="35">
         <v>3378.5009999999993</v>
       </c>
-      <c r="X24" s="36">
+      <c r="X24" s="35">
         <v>723.96449999999982</v>
       </c>
-      <c r="Y24" s="36">
-        <v>0</v>
-      </c>
-      <c r="Z24" s="36">
+      <c r="Y24" s="35">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="35">
         <v>3378.5009999999993</v>
       </c>
-      <c r="AA24" s="36">
+      <c r="AA24" s="35">
         <v>723.96449999999982</v>
       </c>
-      <c r="AB24" s="36">
-        <v>0</v>
-      </c>
-      <c r="AC24" s="36">
+      <c r="AB24" s="35">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="35">
         <v>965.28599999999983</v>
       </c>
       <c r="AE24" s="22">
@@ -3138,7 +3151,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34">
       <c r="B25" s="11">
         <v>2.11</v>
       </c>
@@ -3236,7 +3249,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -3266,40 +3279,40 @@
       <c r="AA26" s="9"/>
       <c r="AB26" s="9"/>
       <c r="AC26" s="9"/>
-      <c r="AE26" s="38"/>
-      <c r="AF26" s="38"/>
+      <c r="AE26" s="37"/>
+      <c r="AF26" s="37"/>
       <c r="AG26" s="9"/>
       <c r="AH26" s="27"/>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34">
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34">
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34">
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34">
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34">
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34">
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:8">
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:8">
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
     </row>

</xml_diff>

<commit_message>
Rearranged contents of input files
</commit_message>
<xml_diff>
--- a/input-FULL-v2.xlsx
+++ b/input-FULL-v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-24560" yWindow="100" windowWidth="24480" windowHeight="14480" tabRatio="699"/>
+    <workbookView xWindow="540" yWindow="380" windowWidth="24480" windowHeight="14480" tabRatio="699"/>
   </bookViews>
   <sheets>
     <sheet name="IMPACT-TECH" sheetId="10" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <author>François Diaz-Maurin</author>
   </authors>
   <commentList>
-    <comment ref="AE3" authorId="0">
+    <comment ref="F3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -40,7 +40,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF3" authorId="0">
+    <comment ref="G3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG3" authorId="0">
+    <comment ref="H3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -200,9 +200,6 @@
     <t>Repackaging of storage casks during offsite storage</t>
   </si>
   <si>
-    <t>Category</t>
-  </si>
-  <si>
     <t>Total cumulative individual worker dose of normal operations during onsite storage</t>
   </si>
   <si>
@@ -309,6 +306,9 @@
   </si>
   <si>
     <t>Public Safety</t>
+  </si>
+  <si>
+    <t>Dimension</t>
   </si>
 </sst>
 </file>
@@ -454,9 +454,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -571,12 +575,16 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="10">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -886,7 +894,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -900,7 +908,7 @@
   <dimension ref="A1:AH34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -910,8 +918,7 @@
     <col min="3" max="3" width="81.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="16.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" style="2" customWidth="1"/>
-    <col min="7" max="8" width="7.33203125" style="7" customWidth="1"/>
+    <col min="6" max="8" width="12.1640625" style="11" customWidth="1"/>
     <col min="9" max="9" width="7.33203125" style="2" customWidth="1"/>
     <col min="10" max="11" width="7.33203125" style="7" customWidth="1"/>
     <col min="12" max="12" width="7.33203125" style="2" customWidth="1"/>
@@ -926,8 +933,9 @@
     <col min="25" max="26" width="7.33203125" style="7" customWidth="1"/>
     <col min="27" max="27" width="7.33203125" style="2" customWidth="1"/>
     <col min="28" max="29" width="7.33203125" style="7" customWidth="1"/>
-    <col min="30" max="30" width="8.83203125" style="3"/>
-    <col min="31" max="33" width="12.1640625" style="2" customWidth="1"/>
+    <col min="30" max="30" width="7.33203125" style="2" customWidth="1"/>
+    <col min="31" max="32" width="7.33203125" style="7" customWidth="1"/>
+    <col min="33" max="33" width="8.83203125" style="3"/>
     <col min="34" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
@@ -937,9 +945,6 @@
       </c>
       <c r="C1" s="16"/>
       <c r="D1" s="17"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
       <c r="I1" s="3"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
@@ -961,52 +966,55 @@
       <c r="AA1" s="3"/>
       <c r="AB1" s="8"/>
       <c r="AC1" s="8"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
     </row>
     <row r="2" spans="1:34" s="14" customFormat="1" ht="30.75" customHeight="1">
-      <c r="F2" s="40" t="s">
+      <c r="I2" s="40" t="s">
         <v>6</v>
-      </c>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40" t="s">
-        <v>16</v>
       </c>
       <c r="J2" s="40"/>
       <c r="K2" s="40"/>
       <c r="L2" s="40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M2" s="40"/>
       <c r="N2" s="40"/>
       <c r="O2" s="40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P2" s="40"/>
       <c r="Q2" s="40"/>
       <c r="R2" s="40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S2" s="40"/>
       <c r="T2" s="40"/>
       <c r="U2" s="40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="V2" s="40"/>
       <c r="W2" s="40"/>
       <c r="X2" s="40" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Y2" s="40"/>
       <c r="Z2" s="40"/>
       <c r="AA2" s="40" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AB2" s="40"/>
       <c r="AC2" s="40"/>
+      <c r="AD2" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE2" s="40"/>
+      <c r="AF2" s="40"/>
     </row>
     <row r="3" spans="1:34" s="1" customFormat="1" ht="28">
       <c r="A3" s="15" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>36</v>
@@ -1021,13 +1029,13 @@
         <v>2</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="I3" s="15" t="s">
         <v>10</v>
@@ -1092,18 +1100,18 @@
       <c r="AC3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="AD3" s="4"/>
+      <c r="AD3" s="15" t="s">
+        <v>10</v>
+      </c>
       <c r="AE3" s="15" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="AF3" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG3" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG3" s="4"/>
+      <c r="AH3" s="15" t="s">
         <v>48</v>
-      </c>
-      <c r="AH3" s="15" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:34">
@@ -1122,23 +1130,23 @@
       <c r="E4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="22">
+        <v>82</v>
+      </c>
+      <c r="G4" s="11">
+        <v>2.1</v>
+      </c>
+      <c r="H4" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="19">
         <v>246</v>
       </c>
-      <c r="G4" s="19">
+      <c r="J4" s="19">
         <v>123</v>
       </c>
-      <c r="H4" s="19">
+      <c r="K4" s="19">
         <v>492</v>
-      </c>
-      <c r="I4" s="19">
-        <v>0</v>
-      </c>
-      <c r="J4" s="19">
-        <v>0</v>
-      </c>
-      <c r="K4" s="19">
-        <v>88</v>
       </c>
       <c r="L4" s="19">
         <v>0</v>
@@ -1150,13 +1158,13 @@
         <v>88</v>
       </c>
       <c r="O4" s="19">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="P4" s="19">
         <v>0</v>
       </c>
       <c r="Q4" s="19">
-        <v>246</v>
+        <v>88</v>
       </c>
       <c r="R4" s="19">
         <v>6</v>
@@ -1168,13 +1176,13 @@
         <v>246</v>
       </c>
       <c r="U4" s="19">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="V4" s="19">
         <v>0</v>
       </c>
       <c r="W4" s="19">
-        <v>88</v>
+        <v>246</v>
       </c>
       <c r="X4" s="19">
         <v>0</v>
@@ -1194,14 +1202,14 @@
       <c r="AC4" s="19">
         <v>88</v>
       </c>
-      <c r="AE4" s="22">
-        <v>82</v>
-      </c>
-      <c r="AF4" s="11">
-        <v>2.1</v>
-      </c>
-      <c r="AG4" s="22" t="b">
-        <v>0</v>
+      <c r="AD4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="19">
+        <v>88</v>
       </c>
       <c r="AH4" s="22">
         <v>400</v>
@@ -1220,23 +1228,23 @@
       <c r="E5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="23">
+        <v>8.2000000000000011</v>
+      </c>
+      <c r="G5" s="11">
+        <v>2.1</v>
+      </c>
+      <c r="H5" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="19">
         <v>24.6</v>
       </c>
-      <c r="G5" s="19">
+      <c r="J5" s="19">
         <v>12.3</v>
       </c>
-      <c r="H5" s="19">
+      <c r="K5" s="19">
         <v>49.2</v>
-      </c>
-      <c r="I5" s="19">
-        <v>0</v>
-      </c>
-      <c r="J5" s="19">
-        <v>0</v>
-      </c>
-      <c r="K5" s="19">
-        <v>8.8000000000000007</v>
       </c>
       <c r="L5" s="19">
         <v>0</v>
@@ -1248,13 +1256,13 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="O5" s="19">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="P5" s="19">
         <v>0</v>
       </c>
       <c r="Q5" s="19">
-        <v>24.6</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="R5" s="19">
         <v>0.6</v>
@@ -1266,13 +1274,13 @@
         <v>24.6</v>
       </c>
       <c r="U5" s="19">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="V5" s="19">
         <v>0</v>
       </c>
       <c r="W5" s="19">
-        <v>8.8000000000000007</v>
+        <v>24.6</v>
       </c>
       <c r="X5" s="19">
         <v>0</v>
@@ -1292,14 +1300,14 @@
       <c r="AC5" s="19">
         <v>8.8000000000000007</v>
       </c>
-      <c r="AE5" s="23">
-        <v>8.2000000000000011</v>
-      </c>
-      <c r="AF5" s="11">
-        <v>2.1</v>
-      </c>
-      <c r="AG5" s="22" t="b">
-        <v>0</v>
+      <c r="AD5" s="19">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="19">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="19">
+        <v>8.8000000000000007</v>
       </c>
       <c r="AH5" s="22">
         <v>400.00000000000011</v>
@@ -1318,14 +1326,11 @@
       <c r="E6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="19">
-        <v>0</v>
-      </c>
-      <c r="G6" s="19">
-        <v>0</v>
-      </c>
-      <c r="H6" s="19">
-        <v>0</v>
+      <c r="F6" s="22">
+        <v>18.756944444444446</v>
+      </c>
+      <c r="H6" s="22" t="b">
+        <v>1</v>
       </c>
       <c r="I6" s="19">
         <v>0</v>
@@ -1334,7 +1339,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="19">
-        <v>112.54166666666667</v>
+        <v>0</v>
       </c>
       <c r="L6" s="19">
         <v>0</v>
@@ -1390,12 +1395,14 @@
       <c r="AC6" s="19">
         <v>112.54166666666667</v>
       </c>
-      <c r="AE6" s="22">
-        <v>18.756944444444446</v>
-      </c>
-      <c r="AF6" s="11"/>
-      <c r="AG6" s="22" t="b">
-        <v>1</v>
+      <c r="AD6" s="19">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="19">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="19">
+        <v>112.54166666666667</v>
       </c>
       <c r="AH6" s="22">
         <v>400</v>
@@ -1414,23 +1421,21 @@
       <c r="E7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="19">
-        <v>0</v>
-      </c>
-      <c r="G7" s="19">
-        <v>0</v>
-      </c>
-      <c r="H7" s="19">
-        <v>0</v>
+      <c r="F7" s="22">
+        <v>108.66666666666667</v>
+      </c>
+      <c r="G7" s="26"/>
+      <c r="H7" s="22" t="b">
+        <v>1</v>
       </c>
       <c r="I7" s="19">
-        <v>246</v>
+        <v>0</v>
       </c>
       <c r="J7" s="19">
-        <v>246</v>
+        <v>0</v>
       </c>
       <c r="K7" s="19">
-        <v>326</v>
+        <v>0</v>
       </c>
       <c r="L7" s="19">
         <v>246</v>
@@ -1466,32 +1471,34 @@
         <v>246</v>
       </c>
       <c r="W7" s="19">
-        <v>652</v>
+        <v>326</v>
       </c>
       <c r="X7" s="19">
-        <v>492</v>
+        <v>246</v>
       </c>
       <c r="Y7" s="19">
-        <v>492</v>
+        <v>246</v>
       </c>
       <c r="Z7" s="19">
         <v>652</v>
       </c>
       <c r="AA7" s="19">
-        <v>246</v>
+        <v>492</v>
       </c>
       <c r="AB7" s="19">
-        <v>246</v>
+        <v>492</v>
       </c>
       <c r="AC7" s="19">
         <v>652</v>
       </c>
-      <c r="AE7" s="22">
-        <v>108.66666666666667</v>
-      </c>
-      <c r="AF7" s="26"/>
-      <c r="AG7" s="22" t="b">
-        <v>1</v>
+      <c r="AD7" s="19">
+        <v>246</v>
+      </c>
+      <c r="AE7" s="19">
+        <v>246</v>
+      </c>
+      <c r="AF7" s="19">
+        <v>652</v>
       </c>
       <c r="AH7" s="22">
         <v>400</v>
@@ -1510,23 +1517,20 @@
       <c r="E8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="19">
-        <v>0</v>
-      </c>
-      <c r="G8" s="19">
-        <v>0</v>
-      </c>
-      <c r="H8" s="19">
+      <c r="F8" s="22">
+        <v>67.333333333333329</v>
+      </c>
+      <c r="H8" s="22" t="b">
         <v>0</v>
       </c>
       <c r="I8" s="19">
-        <v>246</v>
+        <v>0</v>
       </c>
       <c r="J8" s="19">
-        <v>123</v>
+        <v>0</v>
       </c>
       <c r="K8" s="19">
-        <v>404</v>
+        <v>0</v>
       </c>
       <c r="L8" s="19">
         <v>246</v>
@@ -1538,13 +1542,13 @@
         <v>404</v>
       </c>
       <c r="O8" s="19">
-        <v>0</v>
+        <v>246</v>
       </c>
       <c r="P8" s="19">
-        <v>0</v>
+        <v>123</v>
       </c>
       <c r="Q8" s="19">
-        <v>0</v>
+        <v>404</v>
       </c>
       <c r="R8" s="19">
         <v>0</v>
@@ -1556,13 +1560,13 @@
         <v>0</v>
       </c>
       <c r="U8" s="19">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="V8" s="19">
         <v>0</v>
       </c>
       <c r="W8" s="19">
-        <v>197.5</v>
+        <v>0</v>
       </c>
       <c r="X8" s="19">
         <v>6</v>
@@ -1582,12 +1586,14 @@
       <c r="AC8" s="19">
         <v>197.5</v>
       </c>
-      <c r="AE8" s="22">
-        <v>67.333333333333329</v>
-      </c>
-      <c r="AF8" s="11"/>
-      <c r="AG8" s="22" t="b">
-        <v>0</v>
+      <c r="AD8" s="19">
+        <v>6</v>
+      </c>
+      <c r="AE8" s="19">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="19">
+        <v>197.5</v>
       </c>
       <c r="AH8" s="22">
         <v>400</v>
@@ -1606,23 +1612,20 @@
       <c r="E9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="19">
-        <v>0</v>
-      </c>
-      <c r="G9" s="19">
-        <v>0</v>
-      </c>
-      <c r="H9" s="19">
+      <c r="F9" s="23">
+        <v>7.3999999999999995</v>
+      </c>
+      <c r="H9" s="22" t="b">
         <v>0</v>
       </c>
       <c r="I9" s="19">
-        <v>21.05</v>
+        <v>0</v>
       </c>
       <c r="J9" s="19">
-        <v>8.8000000000000007</v>
+        <v>0</v>
       </c>
       <c r="K9" s="19">
-        <v>44.4</v>
+        <v>0</v>
       </c>
       <c r="L9" s="19">
         <v>21.05</v>
@@ -1634,13 +1637,13 @@
         <v>44.4</v>
       </c>
       <c r="O9" s="19">
-        <v>0</v>
+        <v>21.05</v>
       </c>
       <c r="P9" s="19">
-        <v>0</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="Q9" s="19">
-        <v>0</v>
+        <v>44.4</v>
       </c>
       <c r="R9" s="19">
         <v>0</v>
@@ -1658,7 +1661,7 @@
         <v>0</v>
       </c>
       <c r="W9" s="19">
-        <v>8.8000000000000007</v>
+        <v>0</v>
       </c>
       <c r="X9" s="19">
         <v>0</v>
@@ -1676,14 +1679,16 @@
         <v>0</v>
       </c>
       <c r="AC9" s="19">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="AD9" s="19">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="19">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="19">
         <v>19.75</v>
-      </c>
-      <c r="AE9" s="23">
-        <v>7.3999999999999995</v>
-      </c>
-      <c r="AF9" s="11"/>
-      <c r="AG9" s="22" t="b">
-        <v>0</v>
       </c>
       <c r="AH9" s="22">
         <v>400</v>
@@ -1691,13 +1696,13 @@
     </row>
     <row r="10" spans="1:34" ht="28">
       <c r="A10" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>30</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>4</v>
@@ -1705,23 +1710,23 @@
       <c r="E10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="24">
+        <v>42.804312846701158</v>
+      </c>
+      <c r="G10" s="9">
+        <v>2.1</v>
+      </c>
+      <c r="H10" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="20">
         <v>188.2264911765335</v>
       </c>
-      <c r="G10" s="20">
+      <c r="J10" s="20">
         <v>135.65614184198367</v>
       </c>
-      <c r="H10" s="20">
+      <c r="K10" s="20">
         <v>271.46217659314192</v>
-      </c>
-      <c r="I10" s="20">
-        <v>31.213587359251484</v>
-      </c>
-      <c r="J10" s="20">
-        <v>16.647246591600791</v>
-      </c>
-      <c r="K10" s="20">
-        <v>98.385010595337349</v>
       </c>
       <c r="L10" s="20">
         <v>31.213587359251484</v>
@@ -1733,13 +1738,13 @@
         <v>98.385010595337349</v>
       </c>
       <c r="O10" s="20">
-        <v>55.915237983009199</v>
+        <v>31.213587359251484</v>
       </c>
       <c r="P10" s="20">
-        <v>14.636299512934926</v>
+        <v>16.647246591600791</v>
       </c>
       <c r="Q10" s="20">
-        <v>186.06996646088254</v>
+        <v>98.385010595337349</v>
       </c>
       <c r="R10" s="20">
         <v>55.915237983009199</v>
@@ -1751,13 +1756,13 @@
         <v>186.06996646088254</v>
       </c>
       <c r="U10" s="20">
-        <v>31.213587359251484</v>
+        <v>55.915237983009199</v>
       </c>
       <c r="V10" s="20">
-        <v>16.647246591600791</v>
+        <v>14.636299512934926</v>
       </c>
       <c r="W10" s="20">
-        <v>98.385010595337349</v>
+        <v>186.06996646088254</v>
       </c>
       <c r="X10" s="20">
         <v>31.213587359251484</v>
@@ -1777,14 +1782,14 @@
       <c r="AC10" s="20">
         <v>98.385010595337349</v>
       </c>
-      <c r="AE10" s="24">
-        <v>42.804312846701158</v>
-      </c>
-      <c r="AF10" s="9">
-        <v>2.1</v>
-      </c>
-      <c r="AG10" s="24" t="b">
-        <v>0</v>
+      <c r="AD10" s="20">
+        <v>31.213587359251484</v>
+      </c>
+      <c r="AE10" s="20">
+        <v>16.647246591600791</v>
+      </c>
+      <c r="AF10" s="20">
+        <v>98.385010595337349</v>
       </c>
       <c r="AH10" s="24">
         <v>322.33425568694531</v>
@@ -1795,7 +1800,7 @@
         <v>31</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>4</v>
@@ -1803,23 +1808,20 @@
       <c r="E11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="13">
-        <v>0</v>
-      </c>
-      <c r="G11" s="13">
-        <v>0</v>
-      </c>
-      <c r="H11" s="13">
+      <c r="F11" s="22">
+        <v>18.432631843244064</v>
+      </c>
+      <c r="H11" s="22" t="b">
         <v>0</v>
       </c>
       <c r="I11" s="13">
-        <v>65.942414458198684</v>
+        <v>0</v>
       </c>
       <c r="J11" s="13">
-        <v>34.981121507539875</v>
+        <v>0</v>
       </c>
       <c r="K11" s="13">
-        <v>110.59579105946439</v>
+        <v>0</v>
       </c>
       <c r="L11" s="13">
         <v>65.942414458198684</v>
@@ -1831,13 +1833,13 @@
         <v>110.59579105946439</v>
       </c>
       <c r="O11" s="13">
-        <v>0</v>
+        <v>65.942414458198684</v>
       </c>
       <c r="P11" s="13">
-        <v>0</v>
+        <v>34.981121507539875</v>
       </c>
       <c r="Q11" s="13">
-        <v>0</v>
+        <v>110.59579105946439</v>
       </c>
       <c r="R11" s="13">
         <v>0</v>
@@ -1849,13 +1851,13 @@
         <v>0</v>
       </c>
       <c r="U11" s="13">
-        <v>18.70681073240435</v>
+        <v>0</v>
       </c>
       <c r="V11" s="13">
-        <v>4.8834024425892553</v>
+        <v>0</v>
       </c>
       <c r="W11" s="13">
-        <v>52.860997784217616</v>
+        <v>0</v>
       </c>
       <c r="X11" s="13">
         <v>18.70681073240435</v>
@@ -1873,14 +1875,16 @@
         <v>4.8834024425892553</v>
       </c>
       <c r="AC11" s="13">
+        <v>52.860997784217616</v>
+      </c>
+      <c r="AD11" s="13">
+        <v>18.70681073240435</v>
+      </c>
+      <c r="AE11" s="13">
+        <v>4.8834024425892553</v>
+      </c>
+      <c r="AF11" s="13">
         <v>52.964378789812258</v>
-      </c>
-      <c r="AE11" s="22">
-        <v>18.432631843244064</v>
-      </c>
-      <c r="AF11" s="11"/>
-      <c r="AG11" s="22" t="b">
-        <v>0</v>
       </c>
       <c r="AH11" s="22">
         <v>400</v>
@@ -1891,7 +1895,7 @@
         <v>32</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>4</v>
@@ -1899,23 +1903,23 @@
       <c r="E12" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="13">
-        <v>0</v>
-      </c>
-      <c r="G12" s="13">
-        <v>0</v>
-      </c>
-      <c r="H12" s="13">
-        <v>0</v>
-      </c>
-      <c r="I12" s="5">
-        <v>2.8580566538344852</v>
-      </c>
-      <c r="J12" s="5">
-        <v>1.9053711025563238</v>
-      </c>
-      <c r="K12" s="5">
-        <v>5.0500079628728587</v>
+      <c r="F12" s="23">
+        <v>2.0518847990169338</v>
+      </c>
+      <c r="G12" s="11">
+        <v>1.4</v>
+      </c>
+      <c r="H12" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="13">
+        <v>0</v>
+      </c>
+      <c r="J12" s="13">
+        <v>0</v>
+      </c>
+      <c r="K12" s="13">
+        <v>0</v>
       </c>
       <c r="L12" s="5">
         <v>2.8580566538344852</v>
@@ -1927,13 +1931,13 @@
         <v>5.0500079628728587</v>
       </c>
       <c r="O12" s="5">
-        <v>1.6213242004549777</v>
+        <v>2.8580566538344852</v>
       </c>
       <c r="P12" s="5">
-        <v>1.0808828003033188</v>
+        <v>1.9053711025563238</v>
       </c>
       <c r="Q12" s="5">
-        <v>2.8647788040559505</v>
+        <v>5.0500079628728587</v>
       </c>
       <c r="R12" s="5">
         <v>1.6213242004549777</v>
@@ -1945,40 +1949,40 @@
         <v>2.8647788040559505</v>
       </c>
       <c r="U12" s="5">
+        <v>1.6213242004549777</v>
+      </c>
+      <c r="V12" s="5">
+        <v>1.0808828003033188</v>
+      </c>
+      <c r="W12" s="5">
+        <v>2.8647788040559505</v>
+      </c>
+      <c r="X12" s="5">
         <v>3.4837982707235353</v>
       </c>
-      <c r="V12" s="5">
+      <c r="Y12" s="5">
         <v>2.3225321804823573</v>
-      </c>
-      <c r="W12" s="5">
-        <v>12.311308794101603</v>
-      </c>
-      <c r="X12" s="5">
-        <v>6.9675965414470706</v>
-      </c>
-      <c r="Y12" s="5">
-        <v>4.6450643609647146</v>
       </c>
       <c r="Z12" s="5">
         <v>12.311308794101603</v>
       </c>
       <c r="AA12" s="5">
-        <v>3.4837982707235353</v>
+        <v>6.9675965414470706</v>
       </c>
       <c r="AB12" s="5">
-        <v>2.3225321804823573</v>
+        <v>4.6450643609647146</v>
       </c>
       <c r="AC12" s="5">
         <v>12.311308794101603</v>
       </c>
-      <c r="AE12" s="23">
-        <v>2.0518847990169338</v>
-      </c>
-      <c r="AF12" s="11">
-        <v>1.4</v>
-      </c>
-      <c r="AG12" s="22" t="b">
-        <v>0</v>
+      <c r="AD12" s="5">
+        <v>3.4837982707235353</v>
+      </c>
+      <c r="AE12" s="5">
+        <v>2.3225321804823573</v>
+      </c>
+      <c r="AF12" s="5">
+        <v>12.311308794101603</v>
       </c>
       <c r="AH12" s="22">
         <v>400</v>
@@ -1989,7 +1993,7 @@
         <v>33</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>3</v>
@@ -1997,84 +2001,83 @@
       <c r="E13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="10">
-        <v>0</v>
-      </c>
-      <c r="G13" s="10">
-        <v>0</v>
-      </c>
-      <c r="H13" s="10">
-        <v>0</v>
-      </c>
-      <c r="I13" s="12">
+      <c r="F13" s="22">
+        <v>92.570416666666645</v>
+      </c>
+      <c r="H13" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="10">
+        <v>0</v>
+      </c>
+      <c r="J13" s="10">
+        <v>0</v>
+      </c>
+      <c r="K13" s="10">
+        <v>0</v>
+      </c>
+      <c r="L13" s="12">
         <v>58.304998124999997</v>
       </c>
-      <c r="J13" s="12">
-        <v>0</v>
-      </c>
-      <c r="K13" s="12">
+      <c r="M13" s="12">
+        <v>0</v>
+      </c>
+      <c r="N13" s="12">
         <v>83.313374999999994</v>
       </c>
-      <c r="L13" s="12">
+      <c r="O13" s="12">
         <v>172.26476718749998</v>
       </c>
-      <c r="M13" s="12">
+      <c r="P13" s="12">
         <v>68.087137499999997</v>
       </c>
-      <c r="N13" s="12">
+      <c r="Q13" s="12">
         <v>277.71124999999995</v>
       </c>
-      <c r="O13" s="13">
+      <c r="R13" s="13">
         <v>66.255679687500006</v>
       </c>
-      <c r="P13" s="13">
+      <c r="S13" s="13">
         <v>45.391424999999998</v>
       </c>
-      <c r="Q13" s="13">
+      <c r="T13" s="13">
         <v>83.313374999999994</v>
       </c>
-      <c r="R13" s="13">
+      <c r="U13" s="13">
         <v>92.757951562499997</v>
       </c>
-      <c r="S13" s="13">
+      <c r="V13" s="13">
         <v>68.087137499999997</v>
       </c>
-      <c r="T13" s="13">
+      <c r="W13" s="13">
         <v>111.08449999999999</v>
       </c>
-      <c r="U13" s="13">
+      <c r="X13" s="13">
         <v>58.304998124999997</v>
       </c>
-      <c r="V13" s="13">
+      <c r="Y13" s="13">
         <v>45.391424999999998</v>
       </c>
-      <c r="W13" s="13">
+      <c r="Z13" s="13">
         <v>83.313374999999994</v>
       </c>
-      <c r="X13" s="13">
+      <c r="AA13" s="13">
         <v>87.457497187499996</v>
-      </c>
-      <c r="Y13" s="13">
-        <v>68.087137499999997</v>
-      </c>
-      <c r="Z13" s="13">
-        <v>99.976049999999987</v>
-      </c>
-      <c r="AA13" s="13">
-        <v>304.7761265625</v>
       </c>
       <c r="AB13" s="13">
         <v>68.087137499999997</v>
       </c>
       <c r="AC13" s="13">
+        <v>99.976049999999987</v>
+      </c>
+      <c r="AD13" s="13">
+        <v>304.7761265625</v>
+      </c>
+      <c r="AE13" s="13">
+        <v>68.087137499999997</v>
+      </c>
+      <c r="AF13" s="13">
         <v>555.4224999999999</v>
-      </c>
-      <c r="AE13" s="22">
-        <v>92.570416666666645</v>
-      </c>
-      <c r="AF13" s="11"/>
-      <c r="AG13" s="22" t="b">
-        <v>0</v>
       </c>
       <c r="AH13" s="22">
         <v>400</v>
@@ -2086,7 +2089,7 @@
         <v>34</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>4</v>
@@ -2094,13 +2097,10 @@
       <c r="E14" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="10">
-        <v>0</v>
-      </c>
-      <c r="G14" s="10">
-        <v>0</v>
-      </c>
-      <c r="H14" s="10">
+      <c r="F14" s="25">
+        <v>2.9453507079200237E-4</v>
+      </c>
+      <c r="H14" s="22" t="b">
         <v>0</v>
       </c>
       <c r="I14" s="10">
@@ -2121,14 +2121,14 @@
       <c r="N14" s="10">
         <v>0</v>
       </c>
-      <c r="O14" s="21">
-        <v>1.472675353960012E-3</v>
-      </c>
-      <c r="P14" s="21">
-        <v>1.1781402831680095E-3</v>
-      </c>
-      <c r="Q14" s="21">
-        <v>1.7672104247520141E-3</v>
+      <c r="O14" s="10">
+        <v>0</v>
+      </c>
+      <c r="P14" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="10">
+        <v>0</v>
       </c>
       <c r="R14" s="21">
         <v>1.472675353960012E-3</v>
@@ -2140,13 +2140,13 @@
         <v>1.7672104247520141E-3</v>
       </c>
       <c r="U14" s="21">
-        <v>5.6837137006959858E-4</v>
+        <v>1.472675353960012E-3</v>
       </c>
       <c r="V14" s="21">
-        <v>4.5469709605567887E-4</v>
+        <v>1.1781402831680095E-3</v>
       </c>
       <c r="W14" s="21">
-        <v>6.8204564408351823E-4</v>
+        <v>1.7672104247520141E-3</v>
       </c>
       <c r="X14" s="21">
         <v>5.6837137006959858E-4</v>
@@ -2166,12 +2166,14 @@
       <c r="AC14" s="21">
         <v>6.8204564408351823E-4</v>
       </c>
-      <c r="AE14" s="25">
-        <v>2.9453507079200237E-4</v>
-      </c>
-      <c r="AF14" s="11"/>
-      <c r="AG14" s="22" t="b">
-        <v>0</v>
+      <c r="AD14" s="21">
+        <v>5.6837137006959858E-4</v>
+      </c>
+      <c r="AE14" s="21">
+        <v>4.5469709605567887E-4</v>
+      </c>
+      <c r="AF14" s="21">
+        <v>6.8204564408351823E-4</v>
       </c>
       <c r="AH14" s="22">
         <v>400.00000000000011</v>
@@ -2179,37 +2181,35 @@
     </row>
     <row r="15" spans="1:34">
       <c r="A15" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B15" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="D15" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>52</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="39">
+      <c r="F15" s="24">
+        <v>30</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="39">
         <v>200</v>
       </c>
-      <c r="G15" s="39">
+      <c r="J15" s="39">
         <v>200</v>
       </c>
-      <c r="H15" s="39">
+      <c r="K15" s="39">
         <v>200</v>
-      </c>
-      <c r="I15" s="39">
-        <v>30</v>
-      </c>
-      <c r="J15" s="39">
-        <v>20</v>
-      </c>
-      <c r="K15" s="39">
-        <v>40</v>
       </c>
       <c r="L15" s="39">
         <v>30</v>
@@ -2221,13 +2221,13 @@
         <v>40</v>
       </c>
       <c r="O15" s="39">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="P15" s="39">
         <v>20</v>
       </c>
       <c r="Q15" s="39">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="R15" s="39">
         <v>60</v>
@@ -2239,13 +2239,13 @@
         <v>100</v>
       </c>
       <c r="U15" s="39">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="V15" s="39">
         <v>20</v>
       </c>
       <c r="W15" s="39">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="X15" s="39">
         <v>30</v>
@@ -2265,12 +2265,14 @@
       <c r="AC15" s="39">
         <v>40</v>
       </c>
-      <c r="AE15" s="24">
+      <c r="AD15" s="39">
         <v>30</v>
       </c>
-      <c r="AF15" s="9"/>
-      <c r="AG15" s="24" t="b">
-        <v>0</v>
+      <c r="AE15" s="39">
+        <v>20</v>
+      </c>
+      <c r="AF15" s="39">
+        <v>40</v>
       </c>
       <c r="AH15" s="24">
         <v>267.76859504132233</v>
@@ -2278,25 +2280,22 @@
     </row>
     <row r="16" spans="1:34">
       <c r="B16" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>54</v>
-      </c>
       <c r="D16" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="19">
-        <v>200</v>
-      </c>
-      <c r="G16" s="19">
-        <v>200</v>
-      </c>
-      <c r="H16" s="19">
-        <v>200</v>
+      <c r="F16" s="22">
+        <v>30</v>
+      </c>
+      <c r="H16" s="22" t="b">
+        <v>0</v>
       </c>
       <c r="I16" s="19">
         <v>200</v>
@@ -2308,22 +2307,22 @@
         <v>200</v>
       </c>
       <c r="L16" s="19">
+        <v>200</v>
+      </c>
+      <c r="M16" s="19">
+        <v>200</v>
+      </c>
+      <c r="N16" s="19">
+        <v>200</v>
+      </c>
+      <c r="O16" s="19">
         <v>30</v>
-      </c>
-      <c r="M16" s="19">
-        <v>20</v>
-      </c>
-      <c r="N16" s="19">
-        <v>40</v>
-      </c>
-      <c r="O16" s="19">
-        <v>60</v>
       </c>
       <c r="P16" s="19">
         <v>20</v>
       </c>
       <c r="Q16" s="19">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="R16" s="19">
         <v>60</v>
@@ -2335,13 +2334,13 @@
         <v>100</v>
       </c>
       <c r="U16" s="19">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="V16" s="19">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="W16" s="19">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="X16" s="19">
         <v>90</v>
@@ -2353,20 +2352,22 @@
         <v>140</v>
       </c>
       <c r="AA16" s="19">
+        <v>90</v>
+      </c>
+      <c r="AB16" s="19">
+        <v>40</v>
+      </c>
+      <c r="AC16" s="19">
+        <v>140</v>
+      </c>
+      <c r="AD16" s="19">
         <v>30</v>
       </c>
-      <c r="AB16" s="19">
+      <c r="AE16" s="19">
         <v>20</v>
       </c>
-      <c r="AC16" s="19">
+      <c r="AF16" s="19">
         <v>40</v>
-      </c>
-      <c r="AE16" s="22">
-        <v>30</v>
-      </c>
-      <c r="AF16" s="11"/>
-      <c r="AG16" s="22" t="b">
-        <v>0</v>
       </c>
       <c r="AH16" s="22">
         <v>267.76859504132233</v>
@@ -2377,21 +2378,19 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="C17" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" s="19">
-        <v>0</v>
-      </c>
-      <c r="G17" s="19">
-        <v>0</v>
-      </c>
-      <c r="H17" s="19">
+      <c r="F17" s="22">
+        <v>30</v>
+      </c>
+      <c r="G17" s="30"/>
+      <c r="H17" s="22" t="b">
         <v>0</v>
       </c>
       <c r="I17" s="19">
@@ -2413,13 +2412,13 @@
         <v>0</v>
       </c>
       <c r="O17" s="19">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="P17" s="19">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="19">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="R17" s="19">
         <v>140</v>
@@ -2431,13 +2430,13 @@
         <v>100</v>
       </c>
       <c r="U17" s="19">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="V17" s="19">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="W17" s="19">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="X17" s="19">
         <v>110</v>
@@ -2457,12 +2456,14 @@
       <c r="AC17" s="19">
         <v>60</v>
       </c>
-      <c r="AE17" s="22">
-        <v>30</v>
-      </c>
-      <c r="AF17" s="30"/>
-      <c r="AG17" s="22" t="b">
-        <v>0</v>
+      <c r="AD17" s="19">
+        <v>110</v>
+      </c>
+      <c r="AE17" s="19">
+        <v>160</v>
+      </c>
+      <c r="AF17" s="19">
+        <v>60</v>
       </c>
       <c r="AH17" s="22">
         <v>400</v>
@@ -2470,34 +2471,34 @@
     </row>
     <row r="18" spans="1:34">
       <c r="B18" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>58</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>59</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="31">
+      <c r="F18" s="23">
+        <v>1.9994513922372859</v>
+      </c>
+      <c r="G18" s="11">
+        <v>2.1</v>
+      </c>
+      <c r="H18" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="31">
         <v>9.9321112826514213</v>
       </c>
-      <c r="G18" s="31">
+      <c r="J18" s="31">
         <v>7.7567426067347807</v>
       </c>
-      <c r="H18" s="31">
+      <c r="K18" s="31">
         <v>13.126319087739748</v>
-      </c>
-      <c r="I18" s="31">
-        <v>1.693606752729711</v>
-      </c>
-      <c r="J18" s="31">
-        <v>1.1296107343160331</v>
-      </c>
-      <c r="K18" s="31">
-        <v>2.2576027711433886</v>
       </c>
       <c r="L18" s="31">
         <v>1.693606752729711</v>
@@ -2509,13 +2510,13 @@
         <v>2.2576027711433886</v>
       </c>
       <c r="O18" s="31">
-        <v>3.0482713406259045</v>
+        <v>1.693606752729711</v>
       </c>
       <c r="P18" s="31">
         <v>1.1296107343160331</v>
       </c>
       <c r="Q18" s="31">
-        <v>5.4268186542917594</v>
+        <v>2.2576027711433886</v>
       </c>
       <c r="R18" s="31">
         <v>3.0482713406259045</v>
@@ -2527,13 +2528,13 @@
         <v>5.4268186542917594</v>
       </c>
       <c r="U18" s="31">
-        <v>1.693606752729711</v>
+        <v>3.0482713406259045</v>
       </c>
       <c r="V18" s="31">
         <v>1.1296107343160331</v>
       </c>
       <c r="W18" s="31">
-        <v>2.2576027711433886</v>
+        <v>5.4268186542917594</v>
       </c>
       <c r="X18" s="31">
         <v>1.693606752729711</v>
@@ -2553,14 +2554,14 @@
       <c r="AC18" s="31">
         <v>2.2576027711433886</v>
       </c>
-      <c r="AE18" s="23">
-        <v>1.9994513922372859</v>
-      </c>
-      <c r="AF18" s="11">
-        <v>2.1</v>
-      </c>
-      <c r="AG18" s="22" t="b">
-        <v>0</v>
+      <c r="AD18" s="31">
+        <v>1.693606752729711</v>
+      </c>
+      <c r="AE18" s="31">
+        <v>1.1296107343160331</v>
+      </c>
+      <c r="AF18" s="31">
+        <v>2.2576027711433886</v>
       </c>
       <c r="AH18" s="22">
         <v>283.26511680855992</v>
@@ -2568,25 +2569,25 @@
     </row>
     <row r="19" spans="1:34">
       <c r="B19" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="D19" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>62</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="19">
-        <v>10.594761322080478</v>
-      </c>
-      <c r="G19" s="19">
-        <v>10.594761322080478</v>
-      </c>
-      <c r="H19" s="19">
-        <v>10.594761322080478</v>
+      <c r="F19" s="23">
+        <v>1.5086418788144973</v>
+      </c>
+      <c r="G19" s="11">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H19" s="22" t="b">
+        <v>0</v>
       </c>
       <c r="I19" s="19">
         <v>10.594761322080478</v>
@@ -2597,23 +2598,23 @@
       <c r="K19" s="19">
         <v>10.594761322080478</v>
       </c>
-      <c r="L19" s="31">
+      <c r="L19" s="19">
+        <v>10.594761322080478</v>
+      </c>
+      <c r="M19" s="19">
+        <v>10.594761322080478</v>
+      </c>
+      <c r="N19" s="19">
+        <v>10.594761322080478</v>
+      </c>
+      <c r="O19" s="31">
         <v>2.1113720079402762</v>
-      </c>
-      <c r="M19" s="31">
-        <v>1.5429100491934944</v>
-      </c>
-      <c r="N19" s="31">
-        <v>2.6798339666870583</v>
-      </c>
-      <c r="O19" s="31">
-        <v>3.8018827612146211</v>
       </c>
       <c r="P19" s="31">
         <v>1.5429100491934944</v>
       </c>
       <c r="Q19" s="31">
-        <v>5.6356321148190061</v>
+        <v>2.6798339666870583</v>
       </c>
       <c r="R19" s="31">
         <v>3.8018827612146211</v>
@@ -2625,13 +2626,13 @@
         <v>5.6356321148190061</v>
       </c>
       <c r="U19" s="31">
-        <v>5.1771947764179096</v>
+        <v>3.8018827612146211</v>
       </c>
       <c r="V19" s="31">
-        <v>2.6798339666870583</v>
+        <v>1.5429100491934944</v>
       </c>
       <c r="W19" s="31">
-        <v>7.579159661637874</v>
+        <v>5.6356321148190061</v>
       </c>
       <c r="X19" s="31">
         <v>5.1771947764179096</v>
@@ -2643,22 +2644,22 @@
         <v>7.579159661637874</v>
       </c>
       <c r="AA19" s="31">
+        <v>5.1771947764179096</v>
+      </c>
+      <c r="AB19" s="31">
+        <v>2.6798339666870583</v>
+      </c>
+      <c r="AC19" s="31">
+        <v>7.579159661637874</v>
+      </c>
+      <c r="AD19" s="31">
         <v>2.1113720079402762</v>
       </c>
-      <c r="AB19" s="31">
+      <c r="AE19" s="31">
         <v>1.5429100491934944</v>
       </c>
-      <c r="AC19" s="31">
+      <c r="AF19" s="31">
         <v>2.6798339666870583</v>
-      </c>
-      <c r="AE19" s="23">
-        <v>1.5086418788144973</v>
-      </c>
-      <c r="AF19" s="11">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="AG19" s="22" t="b">
-        <v>0</v>
       </c>
       <c r="AH19" s="22">
         <v>222.46621256208954</v>
@@ -2666,34 +2667,31 @@
     </row>
     <row r="20" spans="1:34">
       <c r="B20" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>64</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>65</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="10">
-        <v>0</v>
-      </c>
-      <c r="G20" s="10">
-        <v>0</v>
-      </c>
-      <c r="H20" s="13">
-        <v>0</v>
-      </c>
-      <c r="I20" s="32">
-        <v>2.8917910447761194E-2</v>
-      </c>
-      <c r="J20" s="32">
-        <v>3.0487804878048777E-3</v>
-      </c>
-      <c r="K20" s="32">
-        <v>0.10016025641025642</v>
+      <c r="F20" s="33">
+        <v>3.3386752136752136E-2</v>
+      </c>
+      <c r="H20" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="10">
+        <v>0</v>
+      </c>
+      <c r="J20" s="10">
+        <v>0</v>
+      </c>
+      <c r="K20" s="13">
+        <v>0</v>
       </c>
       <c r="L20" s="32">
         <v>2.8917910447761194E-2</v>
@@ -2723,13 +2721,13 @@
         <v>0.10016025641025642</v>
       </c>
       <c r="U20" s="32">
-        <v>5.7835820895522388E-2</v>
+        <v>2.8917910447761194E-2</v>
       </c>
       <c r="V20" s="32">
-        <v>6.0975609756097554E-3</v>
+        <v>3.0487804878048777E-3</v>
       </c>
       <c r="W20" s="32">
-        <v>0.20032051282051283</v>
+        <v>0.10016025641025642</v>
       </c>
       <c r="X20" s="32">
         <v>5.7835820895522388E-2</v>
@@ -2749,12 +2747,14 @@
       <c r="AC20" s="32">
         <v>0.20032051282051283</v>
       </c>
-      <c r="AE20" s="33">
-        <v>3.3386752136752136E-2</v>
-      </c>
-      <c r="AF20" s="11"/>
-      <c r="AG20" s="22" t="b">
-        <v>0</v>
+      <c r="AD20" s="32">
+        <v>5.7835820895522388E-2</v>
+      </c>
+      <c r="AE20" s="32">
+        <v>6.0975609756097554E-3</v>
+      </c>
+      <c r="AF20" s="32">
+        <v>0.20032051282051283</v>
       </c>
       <c r="AH20" s="22">
         <v>400</v>
@@ -2762,37 +2762,37 @@
     </row>
     <row r="21" spans="1:34">
       <c r="A21" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="C21" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="D21" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>69</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="34">
+      <c r="F21" s="24">
+        <v>390.2</v>
+      </c>
+      <c r="G21" s="9">
+        <v>2.1</v>
+      </c>
+      <c r="H21" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" s="34">
         <v>2270.6</v>
       </c>
-      <c r="G21" s="34">
+      <c r="J21" s="34">
         <v>2135.3000000000002</v>
       </c>
-      <c r="H21" s="34">
+      <c r="K21" s="34">
         <v>2541.1999999999998</v>
-      </c>
-      <c r="I21" s="34">
-        <v>300</v>
-      </c>
-      <c r="J21" s="34">
-        <v>200</v>
-      </c>
-      <c r="K21" s="34">
-        <v>496.8</v>
       </c>
       <c r="L21" s="34">
         <v>300</v>
@@ -2804,13 +2804,13 @@
         <v>496.8</v>
       </c>
       <c r="O21" s="34">
-        <v>606.6</v>
+        <v>300</v>
       </c>
       <c r="P21" s="34">
         <v>200</v>
       </c>
       <c r="Q21" s="34">
-        <v>1270.5999999999999</v>
+        <v>496.8</v>
       </c>
       <c r="R21" s="34">
         <v>606.6</v>
@@ -2822,13 +2822,13 @@
         <v>1270.5999999999999</v>
       </c>
       <c r="U21" s="34">
-        <v>300</v>
+        <v>606.6</v>
       </c>
       <c r="V21" s="34">
         <v>200</v>
       </c>
       <c r="W21" s="34">
-        <v>496.8</v>
+        <v>1270.5999999999999</v>
       </c>
       <c r="X21" s="34">
         <v>300</v>
@@ -2848,14 +2848,14 @@
       <c r="AC21" s="34">
         <v>496.8</v>
       </c>
-      <c r="AE21" s="24">
-        <v>390.2</v>
-      </c>
-      <c r="AF21" s="9">
-        <v>2.1</v>
-      </c>
-      <c r="AG21" s="24" t="b">
-        <v>0</v>
+      <c r="AD21" s="34">
+        <v>300</v>
+      </c>
+      <c r="AE21" s="34">
+        <v>200</v>
+      </c>
+      <c r="AF21" s="34">
+        <v>496.8</v>
       </c>
       <c r="AH21" s="24">
         <v>291.78003760315778</v>
@@ -2866,91 +2866,90 @@
         <v>2.8</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="35">
-        <v>0</v>
-      </c>
-      <c r="G22" s="35">
-        <v>0</v>
-      </c>
-      <c r="H22" s="35">
+      <c r="F22" s="22">
+        <v>483.59692047184171</v>
+      </c>
+      <c r="H22" s="22" t="b">
         <v>0</v>
       </c>
       <c r="I22" s="35">
+        <v>0</v>
+      </c>
+      <c r="J22" s="35">
+        <v>0</v>
+      </c>
+      <c r="K22" s="35">
+        <v>0</v>
+      </c>
+      <c r="L22" s="35">
         <v>2241.1883561643835</v>
       </c>
-      <c r="J22" s="35">
+      <c r="M22" s="35">
         <v>2005.9383561643835</v>
       </c>
-      <c r="K22" s="35">
+      <c r="N22" s="35">
         <v>2610.6675228310505</v>
       </c>
-      <c r="L22" s="35">
-        <v>0</v>
-      </c>
-      <c r="M22" s="35">
-        <v>0</v>
-      </c>
-      <c r="N22" s="35">
-        <v>0</v>
-      </c>
       <c r="O22" s="35">
+        <v>0</v>
+      </c>
+      <c r="P22" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="35">
+        <v>0</v>
+      </c>
+      <c r="R22" s="35">
         <v>656.73922500000003</v>
       </c>
-      <c r="P22" s="35">
+      <c r="S22" s="35">
         <v>287.28750000000002</v>
       </c>
-      <c r="Q22" s="35">
+      <c r="T22" s="35">
         <v>1333.0139999999999</v>
       </c>
-      <c r="R22" s="35">
-        <v>0</v>
-      </c>
-      <c r="S22" s="35">
-        <v>0</v>
-      </c>
-      <c r="T22" s="35">
-        <v>0</v>
-      </c>
       <c r="U22" s="35">
+        <v>0</v>
+      </c>
+      <c r="V22" s="35">
+        <v>0</v>
+      </c>
+      <c r="W22" s="35">
+        <v>0</v>
+      </c>
+      <c r="X22" s="35">
         <v>1536.8775811643836</v>
       </c>
-      <c r="V22" s="35">
+      <c r="Y22" s="35">
         <v>761.4258561643835</v>
       </c>
-      <c r="W22" s="35">
+      <c r="Z22" s="35">
         <v>2901.5815228310503</v>
       </c>
-      <c r="X22" s="35">
+      <c r="AA22" s="35">
         <v>880.13835616438359</v>
       </c>
-      <c r="Y22" s="35">
+      <c r="AB22" s="35">
         <v>474.13835616438354</v>
       </c>
-      <c r="Z22" s="35">
+      <c r="AC22" s="35">
         <v>1568.5675228310502</v>
       </c>
-      <c r="AA22" s="35">
-        <v>0</v>
-      </c>
-      <c r="AB22" s="35">
-        <v>0</v>
-      </c>
-      <c r="AC22" s="35">
-        <v>0</v>
-      </c>
-      <c r="AE22" s="22">
-        <v>483.59692047184171</v>
-      </c>
-      <c r="AF22" s="11"/>
-      <c r="AG22" s="22" t="b">
+      <c r="AD22" s="35">
+        <v>0</v>
+      </c>
+      <c r="AE22" s="35">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="35">
         <v>0</v>
       </c>
       <c r="AH22" s="22">
@@ -2959,95 +2958,94 @@
     </row>
     <row r="23" spans="1:34">
       <c r="B23" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>72</v>
-      </c>
       <c r="D23" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="35">
-        <v>0</v>
-      </c>
-      <c r="G23" s="35">
-        <v>0</v>
-      </c>
-      <c r="H23" s="35">
-        <v>0</v>
-      </c>
-      <c r="I23" s="36">
+      <c r="F23" s="23">
+        <v>5.3523712391636913</v>
+      </c>
+      <c r="H23" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" s="35">
+        <v>0</v>
+      </c>
+      <c r="J23" s="35">
+        <v>0</v>
+      </c>
+      <c r="K23" s="35">
+        <v>0</v>
+      </c>
+      <c r="L23" s="36">
         <v>6.6497816352588943</v>
       </c>
-      <c r="J23" s="35">
-        <v>0</v>
-      </c>
-      <c r="K23" s="35">
+      <c r="M23" s="35">
+        <v>0</v>
+      </c>
+      <c r="N23" s="35">
         <v>11.496319126452976</v>
       </c>
-      <c r="L23" s="35">
+      <c r="O23" s="35">
         <v>11.220132987701069</v>
       </c>
-      <c r="M23" s="36">
+      <c r="P23" s="36">
         <v>3.4094245332863689</v>
       </c>
-      <c r="N23" s="35">
+      <c r="Q23" s="35">
         <v>21.142655864741108</v>
       </c>
-      <c r="O23" s="36">
+      <c r="R23" s="36">
         <v>7.5565700400669256</v>
       </c>
-      <c r="P23" s="36">
+      <c r="S23" s="36">
         <v>3.6367195021721268</v>
       </c>
-      <c r="Q23" s="35">
+      <c r="T23" s="35">
         <v>11.496319126452976</v>
       </c>
-      <c r="R23" s="36">
+      <c r="U23" s="36">
         <v>6.0416100703005764</v>
       </c>
-      <c r="S23" s="36">
+      <c r="V23" s="36">
         <v>3.4094245332863689</v>
       </c>
-      <c r="T23" s="36">
+      <c r="W23" s="36">
         <v>8.4570623458964427</v>
       </c>
-      <c r="U23" s="36">
+      <c r="X23" s="36">
         <v>5.9121155666607965</v>
       </c>
-      <c r="V23" s="36">
+      <c r="Y23" s="36">
         <v>4.3512386990724439</v>
       </c>
-      <c r="W23" s="36">
+      <c r="Z23" s="36">
         <v>8.9520517787953491</v>
       </c>
-      <c r="X23" s="36">
+      <c r="AA23" s="36">
         <v>4.2165083184599688</v>
       </c>
-      <c r="Y23" s="36">
+      <c r="AB23" s="36">
         <v>2.362283273839878</v>
       </c>
-      <c r="Z23" s="36">
+      <c r="AC23" s="36">
         <v>5.7805609382967873</v>
       </c>
-      <c r="AA23" s="35">
+      <c r="AD23" s="35">
         <v>14.693892624936256</v>
       </c>
-      <c r="AB23" s="36">
+      <c r="AE23" s="36">
         <v>1.7876083630800612</v>
       </c>
-      <c r="AC23" s="35">
+      <c r="AF23" s="35">
         <v>32.114227434982148</v>
-      </c>
-      <c r="AE23" s="23">
-        <v>5.3523712391636913</v>
-      </c>
-      <c r="AF23" s="11"/>
-      <c r="AG23" s="22" t="b">
-        <v>0</v>
       </c>
       <c r="AH23" s="22">
         <v>400</v>
@@ -3055,28 +3053,28 @@
     </row>
     <row r="24" spans="1:34">
       <c r="B24" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>74</v>
-      </c>
       <c r="D24" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="35">
+        <v>55</v>
+      </c>
+      <c r="F24" s="22">
+        <v>804.40499999999986</v>
+      </c>
+      <c r="G24" s="11">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H24" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" s="35">
         <v>4826.4299999999994</v>
-      </c>
-      <c r="G24" s="35">
-        <v>0</v>
-      </c>
-      <c r="H24" s="35">
-        <v>4826.4299999999994</v>
-      </c>
-      <c r="I24" s="35">
-        <v>723.96449999999982</v>
       </c>
       <c r="J24" s="35">
         <v>0</v>
@@ -3091,16 +3089,16 @@
         <v>0</v>
       </c>
       <c r="N24" s="35">
+        <v>4826.4299999999994</v>
+      </c>
+      <c r="O24" s="35">
+        <v>723.96449999999982</v>
+      </c>
+      <c r="P24" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="35">
         <v>965.28599999999983</v>
-      </c>
-      <c r="O24" s="35">
-        <v>1447.9289999999996</v>
-      </c>
-      <c r="P24" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="35">
-        <v>2413.2149999999997</v>
       </c>
       <c r="R24" s="35">
         <v>1447.9289999999996</v>
@@ -3112,13 +3110,13 @@
         <v>2413.2149999999997</v>
       </c>
       <c r="U24" s="35">
-        <v>723.96449999999982</v>
+        <v>1447.9289999999996</v>
       </c>
       <c r="V24" s="35">
         <v>0</v>
       </c>
       <c r="W24" s="35">
-        <v>3378.5009999999993</v>
+        <v>2413.2149999999997</v>
       </c>
       <c r="X24" s="35">
         <v>723.96449999999982</v>
@@ -3136,16 +3134,16 @@
         <v>0</v>
       </c>
       <c r="AC24" s="35">
+        <v>3378.5009999999993</v>
+      </c>
+      <c r="AD24" s="35">
+        <v>723.96449999999982</v>
+      </c>
+      <c r="AE24" s="35">
+        <v>0</v>
+      </c>
+      <c r="AF24" s="35">
         <v>965.28599999999983</v>
-      </c>
-      <c r="AE24" s="22">
-        <v>804.40499999999986</v>
-      </c>
-      <c r="AF24" s="11">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="AG24" s="28" t="b">
-        <v>1</v>
       </c>
       <c r="AH24" s="22">
         <v>400</v>
@@ -3156,22 +3154,22 @@
         <v>2.11</v>
       </c>
       <c r="C25" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="11" t="s">
         <v>75</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>76</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="13">
-        <v>132.42517312500001</v>
-      </c>
-      <c r="G25" s="13">
-        <v>57.45750000000001</v>
-      </c>
-      <c r="H25" s="13">
-        <v>275.22142500000001</v>
+      <c r="F25" s="22">
+        <v>45.870237500000002</v>
+      </c>
+      <c r="G25" s="11">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H25" s="22" t="b">
+        <v>0</v>
       </c>
       <c r="I25" s="13">
         <v>132.42517312500001</v>
@@ -3191,14 +3189,14 @@
       <c r="N25" s="13">
         <v>275.22142500000001</v>
       </c>
-      <c r="O25" s="5">
-        <v>2.3701218749999997</v>
+      <c r="O25" s="13">
+        <v>132.42517312500001</v>
       </c>
       <c r="P25" s="13">
-        <v>0</v>
+        <v>57.45750000000001</v>
       </c>
       <c r="Q25" s="13">
-        <v>17.23725</v>
+        <v>275.22142500000001</v>
       </c>
       <c r="R25" s="5">
         <v>2.3701218749999997</v>
@@ -3210,13 +3208,13 @@
         <v>17.23725</v>
       </c>
       <c r="U25" s="5">
-        <v>3.0165187500000004</v>
+        <v>2.3701218749999997</v>
       </c>
       <c r="V25" s="13">
         <v>0</v>
       </c>
       <c r="W25" s="13">
-        <v>20.684699999999996</v>
+        <v>17.23725</v>
       </c>
       <c r="X25" s="5">
         <v>3.0165187500000004</v>
@@ -3236,14 +3234,14 @@
       <c r="AC25" s="13">
         <v>20.684699999999996</v>
       </c>
-      <c r="AE25" s="22">
-        <v>45.870237500000002</v>
-      </c>
-      <c r="AF25" s="11">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="AG25" s="22" t="b">
-        <v>0</v>
+      <c r="AD25" s="5">
+        <v>3.0165187500000004</v>
+      </c>
+      <c r="AE25" s="13">
+        <v>0</v>
+      </c>
+      <c r="AF25" s="13">
+        <v>20.684699999999996</v>
       </c>
       <c r="AH25" s="22">
         <v>400</v>
@@ -3255,8 +3253,8 @@
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
@@ -3279,56 +3277,56 @@
       <c r="AA26" s="9"/>
       <c r="AB26" s="9"/>
       <c r="AC26" s="9"/>
-      <c r="AE26" s="37"/>
-      <c r="AF26" s="37"/>
-      <c r="AG26" s="9"/>
+      <c r="AD26" s="9"/>
+      <c r="AE26" s="9"/>
+      <c r="AF26" s="9"/>
       <c r="AH26" s="27"/>
     </row>
     <row r="27" spans="1:34">
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
     </row>
     <row r="28" spans="1:34">
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
     </row>
     <row r="29" spans="1:34">
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
     </row>
     <row r="30" spans="1:34">
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
     </row>
     <row r="31" spans="1:34">
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
     </row>
     <row r="32" spans="1:34">
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
     </row>
-    <row r="33" spans="7:8">
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
+    <row r="33" spans="10:11">
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
     </row>
-    <row r="34" spans="7:8">
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
+    <row r="34" spans="10:11">
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="R2:T2"/>
     <mergeCell ref="U2:W2"/>
     <mergeCell ref="X2:Z2"/>
     <mergeCell ref="AA2:AC2"/>
-    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="AD2:AF2"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="R2:T2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="F4:AC4">
+  <conditionalFormatting sqref="I4:AF4">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -3340,7 +3338,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F5:AC5">
+  <conditionalFormatting sqref="I5:AF5">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -3352,7 +3350,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6:AC6">
+  <conditionalFormatting sqref="I6:AF6">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -3364,7 +3362,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7:AC7">
+  <conditionalFormatting sqref="I7:AF7">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -3376,7 +3374,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F8:AC8">
+  <conditionalFormatting sqref="I8:AF8">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -3388,7 +3386,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F9:AC9">
+  <conditionalFormatting sqref="I9:AF9">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -3400,7 +3398,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F10:AC10">
+  <conditionalFormatting sqref="I10:AF10">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -3412,7 +3410,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F11:AC11">
+  <conditionalFormatting sqref="I11:AF11">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -3424,7 +3422,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F13:AC13">
+  <conditionalFormatting sqref="I13:AF13">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -3436,7 +3434,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F14:AC14">
+  <conditionalFormatting sqref="I14:AF14">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -3448,7 +3446,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F12:AC12">
+  <conditionalFormatting sqref="I12:AF12">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -3460,7 +3458,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F15:AC15">
+  <conditionalFormatting sqref="I15:AF15">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -3472,7 +3470,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F16:AC16">
+  <conditionalFormatting sqref="I16:AF16">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -3484,7 +3482,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F18:AC18">
+  <conditionalFormatting sqref="I18:AF18">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -3496,7 +3494,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F19:AC19">
+  <conditionalFormatting sqref="I19:AF19">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -3508,7 +3506,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:AC20">
+  <conditionalFormatting sqref="I20:AF20">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -3520,7 +3518,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F25:AC25">
+  <conditionalFormatting sqref="I25:AF25">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -3532,7 +3530,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F24:AC24">
+  <conditionalFormatting sqref="I24:AF24">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3544,7 +3542,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F23:AC23">
+  <conditionalFormatting sqref="I23:AF23">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -3556,7 +3554,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21:AC21">
+  <conditionalFormatting sqref="I21:AF21">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -3568,7 +3566,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F17:AC17">
+  <conditionalFormatting sqref="I17:AF17">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -3580,7 +3578,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F22:AC22">
+  <conditionalFormatting sqref="I22:AF22">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>